<commit_message>
https://jira.hl7.org/browse/FHIR-51222  "Added EHDS models and maps to profiles"
</commit_message>
<xml_diff>
--- a/_sources/xtehr-model-map.xlsx
+++ b/_sources/xtehr-model-map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="Questa_cartella_di_lavoro" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\hl7eu-base\__r4-r5\input\fsh\models\xtehr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\hl7eu-base-r5\__r4-r5\_sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D669C9-A8AC-4815-91C3-74C82167B201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7479325B-5513-494E-AB2E-9F9AB29A9D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-21710" windowWidth="38620" windowHeight="21100" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-21710" windowWidth="38620" windowHeight="21100" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="humanName" sheetId="1" r:id="rId1"/>
@@ -19,21 +19,23 @@
     <sheet name="patient" sheetId="4" r:id="rId4"/>
     <sheet name="patientAnimal" sheetId="5" r:id="rId5"/>
     <sheet name="telecom" sheetId="6" r:id="rId6"/>
-    <sheet name="address" sheetId="7" r:id="rId7"/>
-    <sheet name="healthProfessional-1" sheetId="9" r:id="rId8"/>
-    <sheet name="healthProfessional-2" sheetId="8" r:id="rId9"/>
+    <sheet name="EHDSAddress" sheetId="7" r:id="rId7"/>
+    <sheet name="EHDSHealthProfessional-1" sheetId="9" r:id="rId8"/>
+    <sheet name="EHDSHealthProfessional-2" sheetId="8" r:id="rId9"/>
+    <sheet name="EHDSBodyStructure" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="Address" localSheetId="6">address!#REF!</definedName>
-    <definedName name="Address.country" localSheetId="6">address!#REF!</definedName>
-    <definedName name="Address.country.extension" localSheetId="6">address!#REF!</definedName>
-    <definedName name="Address.country.extension.2" localSheetId="6">address!#REF!</definedName>
-    <definedName name="Address.country.extension.value_x_" localSheetId="6">address!#REF!</definedName>
-    <definedName name="Address.line" localSheetId="6">address!#REF!</definedName>
-    <definedName name="Address.line.extension" localSheetId="6">address!#REF!</definedName>
-    <definedName name="Address.line.extension.2" localSheetId="6">address!#REF!</definedName>
-    <definedName name="Address.line.extension.3" localSheetId="6">address!#REF!</definedName>
-    <definedName name="Address.line.extension.4" localSheetId="6">address!#REF!</definedName>
+    <definedName name="Address" localSheetId="6">EHDSAddress!#REF!</definedName>
+    <definedName name="Address.country" localSheetId="6">EHDSAddress!#REF!</definedName>
+    <definedName name="Address.country.extension" localSheetId="6">EHDSAddress!#REF!</definedName>
+    <definedName name="Address.country.extension.2" localSheetId="6">EHDSAddress!#REF!</definedName>
+    <definedName name="Address.country.extension.value_x_" localSheetId="6">EHDSAddress!#REF!</definedName>
+    <definedName name="Address.line" localSheetId="6">EHDSAddress!#REF!</definedName>
+    <definedName name="Address.line.extension" localSheetId="6">EHDSAddress!#REF!</definedName>
+    <definedName name="Address.line.extension.2" localSheetId="6">EHDSAddress!#REF!</definedName>
+    <definedName name="Address.line.extension.3" localSheetId="6">EHDSAddress!#REF!</definedName>
+    <definedName name="Address.line.extension.4" localSheetId="6">EHDSAddress!#REF!</definedName>
+    <definedName name="BodyStructure.extension.2" localSheetId="9">EHDSBodyStructure!$C$7</definedName>
     <definedName name="Location.address" localSheetId="1">location!$C$7</definedName>
     <definedName name="Location.managingOrganization" localSheetId="1">location!$C$8</definedName>
     <definedName name="Location.name" localSheetId="1">location!$C$4</definedName>
@@ -71,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="200">
   <si>
     <t>description</t>
   </si>
@@ -620,6 +622,57 @@
   </si>
   <si>
     <t>AddressEu</t>
+  </si>
+  <si>
+    <t>Identifier for this instance of the anatomical structure.</t>
+  </si>
+  <si>
+    <t>morphology</t>
+  </si>
+  <si>
+    <t>locationQualifier</t>
+  </si>
+  <si>
+    <t>laterality</t>
+  </si>
+  <si>
+    <t>The kind of structure being represented by the body structure at BodyStructure.location. This can define both normal and abnormal morphologies.</t>
+  </si>
+  <si>
+    <t>Body site</t>
+  </si>
+  <si>
+    <t>Additional qualifier of the body structure (e.g. upper, lower, left side).</t>
+  </si>
+  <si>
+    <t>Body structure laterality (e.g. left, right)</t>
+  </si>
+  <si>
+    <t>Textual description of the body structure</t>
+  </si>
+  <si>
+    <t>Bodystructure identifier</t>
+  </si>
+  <si>
+    <t>Kind of Structure</t>
+  </si>
+  <si>
+    <t>Body site modifier</t>
+  </si>
+  <si>
+    <t>Body Structure Laterality</t>
+  </si>
+  <si>
+    <t>Text summary of the resource, for human interpretation</t>
+  </si>
+  <si>
+    <t>includedStructure.structure</t>
+  </si>
+  <si>
+    <t>includedStructure.laterality</t>
+  </si>
+  <si>
+    <t>includedStructure.qualifier</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1058,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1161,6 +1214,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2421,6 +2480,174 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A489D46F-1A6F-4633-8374-1E410CDAD2B7}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="25.953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.453125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="28.6796875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="26.90625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="24.08984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="23.1796875" customWidth="1"/>
+    <col min="7" max="7" width="49.6796875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A1" s="58" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="56"/>
+      <c r="E1" s="57"/>
+      <c r="G1"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A2" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="G2"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A3" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="G3"/>
+    </row>
+    <row r="4" spans="1:7" ht="45" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A4" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A5" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="C5" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:7" ht="30.25" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A6" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="C6" s="61" t="s">
+        <v>199</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="G6"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A7" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" s="61" t="s">
+        <v>198</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="G7"/>
+    </row>
+    <row r="8" spans="1:7" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A8" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="G8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Foglio4"/>
@@ -3271,7 +3498,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -3732,7 +3959,7 @@
   <sheetPr codeName="Foglio2"/>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>